<commit_message>
Added space to beginning of unit attribute to identify it as dimension
</commit_message>
<xml_diff>
--- a/QCalc/Resources/quantities.xlsx
+++ b/QCalc/Resources/quantities.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="671" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="671" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -1078,12 +1078,12 @@
   </sheetPr>
   <dimension ref="A1:IR166"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B113" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B104" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A113" activeCellId="0" sqref="A113"/>
-      <selection pane="bottomRight" activeCell="E155" activeCellId="1" sqref="A1:A172 E155"/>
+      <selection pane="bottomLeft" activeCell="A104" activeCellId="0" sqref="A104"/>
+      <selection pane="bottomRight" activeCell="A111" activeCellId="0" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -24818,7 +24818,7 @@
         <v>161</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>15</v>
@@ -30038,7 +30038,7 @@
         <v>187</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>15</v>
@@ -32618,8 +32618,8 @@
   </sheetPr>
   <dimension ref="A1:A172"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A172"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A115" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -33171,7 +33171,7 @@
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="14" t="str">
         <f aca="false">IF(AND(Data!A91&lt;&gt;"",Data!C91="Y"),"type "&amp;Data!A91&amp;"= Quantity(final unit="&amp;CHAR(34)&amp;" "&amp;Data!F91&amp;CHAR(34)&amp;IF(Data!I91&lt;&gt;"",", "&amp;"min="&amp;Data!I91,"")&amp;IF(Data!J91&lt;&gt;"",", "&amp;"max="&amp;Data!J91,"")&amp;") "&amp;IF(Data!B91&lt;&gt;"",CHAR(34)&amp;Data!B91&amp;CHAR(34),"")&amp;";","")</f>
-        <v>type MassSpecific= Quantity(final unit=" M/N", min=0) "Specific mass";</v>
+        <v/>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33291,7 +33291,7 @@
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="14" t="str">
         <f aca="false">IF(AND(Data!A111&lt;&gt;"",Data!C111="Y"),"type "&amp;Data!A111&amp;"= Quantity(final unit="&amp;CHAR(34)&amp;" "&amp;Data!F111&amp;CHAR(34)&amp;IF(Data!I111&lt;&gt;"",", "&amp;"min="&amp;Data!I111,"")&amp;IF(Data!J111&lt;&gt;"",", "&amp;"max="&amp;Data!J111,"")&amp;") "&amp;IF(Data!B111&lt;&gt;"",CHAR(34)&amp;Data!B111&amp;CHAR(34),"")&amp;";","")</f>
-        <v/>
+        <v>type PotentialAbsolute= Quantity(final unit=" L2.M/(N.T2)", min=0) "Absolute potential";</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33679,7 +33679,7 @@
   <dimension ref="A1:A172"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A142" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A1:A172"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -34347,7 +34347,7 @@
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="15" t="str">
         <f aca="false">IF(AND(Data!A91&lt;&gt;"",Data!C91="Y"),"parameter Q."&amp;Data!A91&amp;" "&amp;Data!A91&amp;"= 1"&amp;IF(LEFT(Data!M91,1)&lt;&gt;"1","*"&amp;Data!M91,RIGHT(Data!M91,LEN(Data!M91)-1))&amp;" "&amp;CHAR(34)&amp;IF(Data!B91&lt;&gt;"",Data!B91,Data!A91)&amp;CHAR(34)&amp;";","")</f>
-        <v>parameter Q.MassSpecific MassSpecific= 1*U.g/U.mol "Specific mass";</v>
+        <v/>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34489,11 +34489,9 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="15" t="inlineStr">
+      <c r="A111" s="15" t="str">
         <f aca="false">IF(AND(Data!A111&lt;&gt;"",Data!C111="Y"),"parameter Q."&amp;Data!A111&amp;" "&amp;Data!A111&amp;"= 1"&amp;IF(LEFT(Data!M111,1)&lt;&gt;"1","*"&amp;Data!M111,RIGHT(Data!M111,LEN(Data!M111)-1))&amp;" "&amp;CHAR(34)&amp;IF(Data!B111&lt;&gt;"",Data!B111,Data!A111)&amp;CHAR(34)&amp;";","")</f>
-        <is>
-          <t/>
-        </is>
+        <v>parameter Q.PotentialAbsolute PotentialAbsolute= 1*U.K "Absolute potential";</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34969,7 +34967,7 @@
   <dimension ref="A1:A174"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A144" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A1:A172"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -36259,7 +36257,7 @@
   <dimension ref="A1:A174"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A144" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A1:A172"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -37341,7 +37339,7 @@
   <dimension ref="A1:A200"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A128" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A158" activeCellId="0" sqref="A1:A172"/>
+      <selection pane="topLeft" activeCell="A158" activeCellId="0" sqref="A158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>